<commit_message>
revert dependance IG NOS cc687a159e6876383320a58fb02eb90386d96176
</commit_message>
<xml_diff>
--- a/sd-questionnaire/ig/ValueSet-ror-usage-context-type-vs.xlsx
+++ b/sd-questionnaire/ig/ValueSet-ror-usage-context-type-vs.xlsx
@@ -8,7 +8,7 @@
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Include from UsageContextType" r:id="rId4" sheetId="2"/>
-    <sheet name="Include from TRE_R67-TypeStru" r:id="rId5" sheetId="3"/>
+    <sheet name="Include from TRE-R67-TypeStru" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
@@ -58,7 +58,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-06T13:35:20+00:00</t>
+    <t>2024-02-06T14:49:20+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>